<commit_message>
update and collect new data / 1806
</commit_message>
<xml_diff>
--- a/platform_scrapper/data/fake_cannabis_used_IDs.xlsx
+++ b/platform_scrapper/data/fake_cannabis_used_IDs.xlsx
@@ -508,17 +508,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>TORONTO</t>
+          <t>MISSISSAUGA</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Body and Spirit Cannabis</t>
+          <t>Tough Bud Cannabis</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>361 YONGE ST</t>
+          <t>296 LAKESHORE RD W</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -528,33 +528,33 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>https://bodyandspiritcannabis.com/</t>
+          <t>https://toughbud.ca/shop-missisauga/</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Dutchie</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>5e45c5d96a6aef00702ed11f</t>
-        </is>
-      </c>
+          <t>Buddi</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr">
         <is>
-          <t>['Curbside pickup', 'In-store pickup', 'In-store shopping']</t>
+          <t>['Curbside pickup', 'Delivery', 'In-store pickup', 'In-store shopping', 'Same-day delivery']</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>16478125989</v>
+        <v>19052782222</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>['Delivery']</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr"/>
+          <t>['Delivery serve within 30 km radius', 'Same-day delivery']</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">$40 minimum order </t>
+        </is>
+      </c>
       <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr"/>
       <c r="N2" t="b">

</xml_diff>